<commit_message>
setup new main project in D:\My Documents\Group3Projects\W6 Project\main_project
</commit_message>
<xml_diff>
--- a/W6 Project/Kanen OS Task Distribution.xlsx
+++ b/W6 Project/Kanen OS Task Distribution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t>T001</t>
   </si>
@@ -163,13 +163,25 @@
   </si>
   <si>
     <t>Sebastian Briones</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Create new tables and encode data</t>
+  </si>
+  <si>
+    <t>1 hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +211,22 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,13 +267,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:C46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -760,7 +790,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
         <v>28</v>
       </c>
@@ -771,7 +801,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
         <v>28</v>
       </c>
@@ -782,14 +812,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
         <v>24</v>
       </c>
@@ -800,12 +830,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
         <v>26</v>
       </c>
@@ -816,7 +846,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
         <v>28</v>
       </c>
@@ -827,7 +857,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
         <v>28</v>
       </c>
@@ -838,14 +868,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:4">
       <c r="A44" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
@@ -856,8 +886,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:4">
+      <c r="A46" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -865,6 +895,23 @@
       </c>
       <c r="C46" s="2" t="s">
         <v>48</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update product service and DAOImpl
</commit_message>
<xml_diff>
--- a/W6 Project/Kanen OS Task Distribution.xlsx
+++ b/W6 Project/Kanen OS Task Distribution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>T001</t>
   </si>
@@ -172,16 +172,13 @@
   </si>
   <si>
     <t>Create new tables and encode data</t>
-  </si>
-  <si>
-    <t>1 hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +228,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -267,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -276,6 +280,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:D48"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -890,7 +895,7 @@
       <c r="A46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -904,14 +909,14 @@
       <c r="A48" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>